<commit_message>
DOCS folder for EX2
</commit_message>
<xml_diff>
--- a/DOCS/Algo1Algo2compare.xlsx
+++ b/DOCS/Algo1Algo2compare.xlsx
@@ -132,12 +132,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,7 +423,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -435,7 +435,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -447,7 +447,7 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H1" t="s">
@@ -477,13 +477,13 @@
         <v>4</v>
       </c>
       <c r="H2">
-        <v>700.71588780000002</v>
+        <v>32.103898280000003</v>
       </c>
       <c r="I2">
         <v>35.210131570000001</v>
       </c>
       <c r="J2">
-        <v>32.103898280000003</v>
+        <v>700.71588780000002</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -503,13 +503,13 @@
         <v>5</v>
       </c>
       <c r="H3">
-        <v>697.57450140000003</v>
+        <v>32.104123690000002</v>
       </c>
       <c r="I3">
         <v>35.210338530000001</v>
       </c>
       <c r="J3">
-        <v>32.104123690000002</v>
+        <v>697.57450140000003</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -530,7 +530,7 @@
       </c>
       <c r="H4">
         <f>H2-H3</f>
-        <v>3.1413863999999876</v>
+        <v>-2.2540999999876021E-4</v>
       </c>
       <c r="I4">
         <f>I2-I3</f>
@@ -538,18 +538,18 @@
       </c>
       <c r="J4">
         <f>J2-J3</f>
-        <v>-2.2540999999876021E-4</v>
+        <v>3.1413863999999876</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -558,10 +558,10 @@
       <c r="G7" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="3"/>
+      <c r="I7" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>